<commit_message>
Male 2020 Age-Grade Road Running Standards
</commit_message>
<xml_diff>
--- a/FemaleRoadStd2020.xlsx
+++ b/FemaleRoadStd2020.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alan Jones\Documents\AgeGrade\Age-Grade-Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79478715-6530-4EC4-A1C2-BC11F1491608}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E740AE67-40C0-40E1-AAE6-2EFB5F9AAF46}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3915" yWindow="1740" windowWidth="13410" windowHeight="15450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3120" yWindow="750" windowWidth="13410" windowHeight="15450" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AgeStdFactors" sheetId="2" r:id="rId1"/>
@@ -139,7 +139,7 @@
     <t>2020-06-20</t>
   </si>
   <si>
-    <t>Approved 2020-05-20 by Long Distance Running (LDR) of USA Track&amp;Field (USATF)</t>
+    <t>Approved 2020-05-20 by Masters Long Distance Running (MLDR) of USA Track&amp;Field (USATF)</t>
   </si>
 </sst>
 </file>
@@ -1016,8 +1016,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V108"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView topLeftCell="A94" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
+      <selection activeCell="A108" sqref="A108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8031,7 +8031,7 @@
   <dimension ref="A1:V108"/>
   <sheetViews>
     <sheetView topLeftCell="A82" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
-      <selection activeCell="A102" sqref="A102:A108"/>
+      <selection activeCell="A108" sqref="A108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14916,8 +14916,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:V108"/>
   <sheetViews>
-    <sheetView topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="D97" sqref="D97"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="G104" sqref="G104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Female 2020 Age-Grade Road Running Standards
</commit_message>
<xml_diff>
--- a/FemaleRoadStd2020.xlsx
+++ b/FemaleRoadStd2020.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alan Jones\Documents\AgeGrade\Age-Grade-Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E740AE67-40C0-40E1-AAE6-2EFB5F9AAF46}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BD818179-3ECE-467F-9E0D-5F3C2B5EAD6B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="750" windowWidth="13410" windowHeight="15450" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1950" yWindow="300" windowWidth="13410" windowHeight="15450" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AgeStdFactors" sheetId="2" r:id="rId1"/>

</xml_diff>

<commit_message>
Working Excel file to produce Female Standards
</commit_message>
<xml_diff>
--- a/FemaleRoadStd2020.xlsx
+++ b/FemaleRoadStd2020.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alan Jones\Documents\AgeGrade\Age-Grade-Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D678867F-AA42-41FD-8132-E92AB0580905}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{72BA33D7-4132-49CD-B564-3BE468886917}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="300" windowWidth="13410" windowHeight="15450" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1950" yWindow="300" windowWidth="19905" windowHeight="15450" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AgeStdFactors" sheetId="2" r:id="rId1"/>

</xml_diff>